<commit_message>
LDL + Hydrant truck to Vehicle class, new meshes, and added a coordinate debug
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE422E62-6399-4BBF-8A1E-B6F3784C63B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E3BD0-4DF5-4FB8-B590-B7FCAFE47516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="H23" sqref="H23:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vehicles now turn based on gates + drive backwards when needed. Vehicles also wait for free area before starting to move
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E3BD0-4DF5-4FB8-B590-B7FCAFE47516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02329A81-C297-4002-97BF-402126F40612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Flight_Closure</t>
   </si>
   <si>
-    <t>Attatch_Tug</t>
-  </si>
-  <si>
     <t>PDCS</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Refuel_Finalising</t>
+  </si>
+  <si>
+    <t>Attach_Tug</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:I23"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,25 +561,25 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <v>4</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5">
         <v>14</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5">
         <v>13</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5">
         <v>16</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5">
         <v>10</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="5">
         <v>10</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5">
         <v>30</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5">
         <v>3</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5">
         <v>25</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="5">
         <v>14</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="5">
         <v>2</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="5">
         <v>2</v>
@@ -1245,14 +1245,14 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="str">
         <f>A28</f>
-        <v>Attatch_Tug</v>
+        <v>Attach_Tug</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1275,14 +1275,14 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5">
         <v>2</v>
       </c>
       <c r="C32" s="1" t="str">
         <f>A28</f>
-        <v>Attatch_Tug</v>
+        <v>Attach_Tug</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
Simulation speed refining: Limiting and stopping vehcicle simulations above 32x
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02329A81-C297-4002-97BF-402126F40612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24FBDFC-8B5A-410B-BC67-0DCBBCEC1A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Parking</t>
   </si>
@@ -528,7 +528,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,8 +1254,12 @@
         <f>A28</f>
         <v>Attach_Tug</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H31" s="3">
         <v>550</v>
       </c>

</xml_diff>